<commit_message>
Terminado plan de personal Adicionado Excel plan de Personal Corregido Herramientas y metodos corregido plan de entrenamiento en SPMP falta referenciar el plan de entrenamiento desde el SPMP falta referencia Documento nuevo de excel con plan de personal
</commit_message>
<xml_diff>
--- a/Plan_de_Personal_Especificacion.xlsx
+++ b/Plan_de_Personal_Especificacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="211" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="171" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Integrantes</t>
   </si>
@@ -67,7 +67,7 @@
     <t>Analisis Por Fase</t>
   </si>
   <si>
-    <t>Fase </t>
+    <t>Fase</t>
   </si>
   <si>
     <t>Actividad</t>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Nombres Integrantes</t>
+  </si>
+  <si>
+    <t>Fecha de realizacion</t>
   </si>
   <si>
     <t>SPMP</t>
@@ -98,6 +101,7 @@
   <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -118,6 +122,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <i val="true"/>
@@ -191,7 +196,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -203,6 +208,10 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -287,23 +296,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:F55"/>
+  <dimension ref="B3:G55"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H50" activeCellId="0" pane="topLeft" sqref="H50"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A12" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D23" activeCellId="0" pane="topLeft" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0509803921569"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.8156862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0549019607843"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.2666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.121568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.5450980392157"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.9529411764706"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5294117647059"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.3843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.1254901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -311,7 +321,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="4">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -325,7 +335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -335,7 +345,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -345,7 +355,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
@@ -355,7 +365,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
@@ -365,7 +375,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -375,7 +385,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
@@ -400,15 +410,19 @@
       <c r="F14" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="G14" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="B15" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
+      <c r="G15" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="B16" s="5"/>
@@ -416,6 +430,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
+      <c r="G16" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="B17" s="5"/>
@@ -423,13 +438,15 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
+      <c r="G17" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="B18" s="5"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="B19" s="5"/>
@@ -437,6 +454,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
+      <c r="G19" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="B20" s="5"/>
@@ -444,6 +462,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
+      <c r="G20" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="B21" s="5"/>
@@ -451,6 +470,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
+      <c r="G21" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="B22" s="5"/>
@@ -458,6 +478,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
+      <c r="G22" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="B23" s="5"/>
@@ -465,6 +486,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
+      <c r="G23" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="B24" s="5"/>
@@ -472,6 +494,7 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
+      <c r="G24" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="B25" s="5"/>
@@ -479,6 +502,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
+      <c r="G25" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="B26" s="5"/>
@@ -486,6 +510,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
+      <c r="G26" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="B27" s="5"/>
@@ -493,6 +518,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
+      <c r="G27" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="B28" s="5"/>
@@ -500,6 +526,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
+      <c r="G28" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="B29" s="5"/>
@@ -507,164 +534,227 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="31">
+      <c r="B31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="B32" s="6" t="s">
-        <v>21</v>
+      <c r="B32" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
+      <c r="G32" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
-      <c r="B33" s="6"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
+      <c r="G33" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
-      <c r="B34" s="6"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
+      <c r="G34" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
-      <c r="B35" s="6"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
+      <c r="G35" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
-      <c r="B36" s="6"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
+      <c r="G36" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
-      <c r="B37" s="6"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
+      <c r="G37" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
-      <c r="B38" s="6"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
+      <c r="G38" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
-      <c r="B39" s="6"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
+      <c r="G39" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
-      <c r="B40" s="6"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
+      <c r="G40" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
-      <c r="B41" s="6"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
+      <c r="G41" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
-      <c r="B42" s="6"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="44">
+      <c r="B44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
-      <c r="B45" s="7" t="s">
-        <v>22</v>
+      <c r="B45" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
+      <c r="G45" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
-      <c r="B46" s="7"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
+      <c r="G46" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
-      <c r="B47" s="7"/>
+      <c r="B47" s="9"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
+      <c r="G47" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
-      <c r="B48" s="7"/>
+      <c r="B48" s="9"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
+      <c r="G48" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
-      <c r="B49" s="7"/>
+      <c r="B49" s="9"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
+      <c r="G49" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
-      <c r="B50" s="7"/>
+      <c r="B50" s="9"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
+      <c r="G50" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
-      <c r="B51" s="7"/>
+      <c r="B51" s="9"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
+      <c r="G51" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
-      <c r="B52" s="7"/>
+      <c r="B52" s="9"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
+      <c r="G52" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
-      <c r="B53" s="7"/>
+      <c r="B53" s="9"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
+      <c r="G53" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
-      <c r="B54" s="7"/>
+      <c r="B54" s="9"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
+      <c r="G54" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
-      <c r="B55" s="7"/>
+      <c r="B55" s="9"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
+      <c r="G55" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -691,17 +781,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -716,17 +806,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>